<commit_message>
update: backlog - grámtica
</commit_message>
<xml_diff>
--- a/Documentacao/Gr08-PlanoRisco.xlsx
+++ b/Documentacao/Gr08-PlanoRisco.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Repositório-UMITRIX\UMITRIX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Repositório-UMITRIX\UMITRIX\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -141,9 +141,6 @@
     <t>Verificação diária por todos membros na organização da ferramenta de gestão (Trello).</t>
   </si>
   <si>
-    <t>Auxílio em tarefas tecnicamente mais complexas  por membros com mais experiência em certa ferramenta ou recurso.</t>
-  </si>
-  <si>
     <t>Ocorrer empecilhos por conta de mal-funcionamento de aparelhos eletrônicos</t>
   </si>
   <si>
@@ -175,6 +172,9 @@
   </si>
   <si>
     <t>Dificuldade de comunicação entre a equipe</t>
+  </si>
+  <si>
+    <t>Auxílio em tarefas tecnicamente mais complexas por membros com mais experiência em certa ferramenta ou recurso.</t>
   </si>
 </sst>
 </file>
@@ -378,9 +378,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -390,19 +387,22 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -745,7 +745,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -761,15 +761,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="76.5" customHeight="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" spans="1:14" s="4" customFormat="1" ht="17.5" customHeight="1" thickBot="1">
       <c r="A2" s="3"/>
@@ -781,25 +781,25 @@
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="87.5" customHeight="1" thickBot="1">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="13" t="s">
+      <c r="C3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -826,11 +826,11 @@
       <c r="G4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="K4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
       <c r="N4" s="19"/>
     </row>
     <row r="5" spans="1:14" s="2" customFormat="1" ht="50" customHeight="1" thickBot="1">
@@ -856,16 +856,16 @@
       <c r="G5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="K5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="16">
+      <c r="L5" s="14">
         <v>3</v>
       </c>
-      <c r="M5" s="17">
+      <c r="M5" s="15">
         <v>6</v>
       </c>
-      <c r="N5" s="17">
+      <c r="N5" s="15">
         <v>9</v>
       </c>
     </row>
@@ -890,7 +890,7 @@
         <v>23</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>9</v>
@@ -910,7 +910,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="6">
         <v>1</v>
@@ -955,7 +955,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="6">
-        <f t="shared" ref="E5:E15" si="0">C8*D8</f>
+        <f t="shared" ref="E8:E15" si="0">C8*D8</f>
         <v>3</v>
       </c>
       <c r="F8" s="6" t="s">
@@ -964,7 +964,7 @@
       <c r="G8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="11"/>
+      <c r="K8" s="10"/>
       <c r="L8" s="6" t="s">
         <v>11</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="6">
         <v>2</v>
@@ -1044,7 +1044,7 @@
         <v>15</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="2" customFormat="1" ht="50" customHeight="1" thickBot="1">
@@ -1052,7 +1052,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="6">
         <v>2</v>
@@ -1068,7 +1068,7 @@
         <v>20</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="2" customFormat="1" ht="50" customHeight="1" thickBot="1">
@@ -1076,7 +1076,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="6">
         <v>2</v>
@@ -1092,7 +1092,7 @@
         <v>23</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="2" customFormat="1" ht="50" customHeight="1" thickBot="1">
@@ -1100,7 +1100,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="6">
         <v>2</v>
@@ -1116,7 +1116,7 @@
         <v>20</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="2" customFormat="1" ht="50" customHeight="1" thickBot="1">
@@ -1124,7 +1124,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="6">
         <v>2</v>
@@ -1140,7 +1140,7 @@
         <v>15</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1162,15 +1162,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD11765F9AC0004AAF0A4CAAFDFAF16A" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="936353fbdaa3cfa0ada3a067af0b2a91">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9fdc8751-6fef-42ec-b05c-835dd8c535b4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5658a1d30780e9e89567900e1bf7d795" ns3:_="">
     <xsd:import namespace="9fdc8751-6fef-42ec-b05c-835dd8c535b4"/>
@@ -1326,6 +1317,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A85FC0E-79F7-49E8-92C5-C8EEEF04D224}">
   <ds:schemaRefs>
@@ -1343,14 +1343,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97071F1C-8CB5-4BD1-B0E1-1BFA8268E317}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F454524-A766-4E67-8148-69B670E55CE3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1366,4 +1358,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97071F1C-8CB5-4BD1-B0E1-1BFA8268E317}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>